<commit_message>
ctrl clicking each artist
</commit_message>
<xml_diff>
--- a/songDataTabe.xlsx
+++ b/songDataTabe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anuraag\Documents\UiPath\SwiftTune1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1B0376-3630-40F4-8A69-38F923E7BEDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29F56227-AFB4-43CA-B9AF-8D27DDB61C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="3900" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Coldplay</t>
+  </si>
+  <si>
+    <t>Parachutes</t>
+  </si>
+  <si>
+    <t>head first</t>
+  </si>
+  <si>
+    <t>Christian French</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>Ellie Goulding</t>
+  </si>
+  <si>
+    <t>Brightest Blue</t>
+  </si>
   <si>
     <t></t>
   </si>
@@ -39,6 +66,9 @@
     <t>WHEN WE ALL FALL ASLEEP, WHERE DO WE GO?</t>
   </si>
   <si>
+    <t>4 hours ago</t>
+  </si>
+  <si>
     <t>Cheap Thrills</t>
   </si>
   <si>
@@ -90,22 +120,7 @@
     <t>Bars and Melody</t>
   </si>
   <si>
-    <t>In My Blood</t>
-  </si>
-  <si>
-    <t>Shawn Mendes</t>
-  </si>
-  <si>
-    <t>Someone Like You</t>
-  </si>
-  <si>
-    <t>Adele</t>
-  </si>
-  <si>
-    <t>an hour ago</t>
-  </si>
-  <si>
-    <t>2 hours ago</t>
+    <t>5 hours ago</t>
   </si>
 </sst>
 </file>
@@ -434,140 +449,147 @@
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H1" s="1"/>
       <c r="I1" s="1">
         <v>0.13472222222222222</v>
       </c>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H2" s="1"/>
       <c r="I2" s="1">
         <v>0.14722222222222223</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1">
         <v>0.16527777777777777</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1">
         <v>0.1361111111111111</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="1">
         <v>0.1423611111111111</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1">
         <v>0.18194444444444444</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H7" s="1"/>
       <c r="I7" s="1">
         <v>0.1173611111111111</v>
       </c>
@@ -577,16 +599,16 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.18541666666666667</v>
       </c>
       <c r="I8" s="1">
         <v>0.14652777777777778</v>
@@ -597,22 +619,37 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.1076388888888889</v>
       </c>
       <c r="I9" s="1">
         <v>0.19791666666666666</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.16041666666666668</v>
+      </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>